<commit_message>
Update Database design in excel
</commit_message>
<xml_diff>
--- a/database/Database-In-More-Detail.xlsx
+++ b/database/Database-In-More-Detail.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\Book-Shop-API\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A0BAE0C-94C1-42E4-9D6F-D7B2BD5511FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5092BAC2-8D74-4914-A2E6-2133F8539C1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{DBAE516F-9EAD-4516-8555-9494F8FA5157}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="128">
   <si>
     <t>Publisher</t>
   </si>
@@ -156,9 +156,6 @@
     <t>Giá tiền ở thời điểm hiện tại</t>
   </si>
   <si>
-    <t>URL hình ảnh</t>
-  </si>
-  <si>
     <t>Mã isbn</t>
   </si>
   <si>
@@ -279,9 +276,6 @@
     <t>NOT NULL, DEFAULT = SYSDATETIME()</t>
   </si>
   <si>
-    <t>Mã nhân viên</t>
-  </si>
-  <si>
     <t>Mã khách hàng</t>
   </si>
   <si>
@@ -294,9 +288,6 @@
     <t>Tổng tiền khách phải trả</t>
   </si>
   <si>
-    <t>NOT NULL, DEFAULT = 1</t>
-  </si>
-  <si>
     <t>PK, FK</t>
   </si>
   <si>
@@ -403,9 +394,6 @@
   </si>
   <si>
     <t>Tiền ship (nếu mua online), còn mua tại store thì ship = 0</t>
-  </si>
-  <si>
-    <t>NOT NULL, default = 0.0</t>
   </si>
   <si>
     <t>paymentMethod</t>
@@ -421,10 +409,19 @@
 2.2. Còn nếu khách mới hoàn toàn thì cứ tạo như thường</t>
   </si>
   <si>
-    <t>Phương thức thanh toán</t>
-  </si>
-  <si>
-    <t>Trạng thái hóa đơn</t>
+    <t>URL hình ảnh (lưu ở server, đừng lấy link onl)</t>
+  </si>
+  <si>
+    <t>Mã nhân viên (cho phép null nếu khách mua onl)</t>
+  </si>
+  <si>
+    <t>Phương thức thanh toán ("Tiền mặt", "Chuyển khoản", "POS",…) lưu dữ liệu giống như vậy để dễ quản lý</t>
+  </si>
+  <si>
+    <t>DEFAULT = 0.0</t>
+  </si>
+  <si>
+    <t>Trạng thái hóa đơn ("Thành công", "Đang vận chuyển", "Lỗi",…) lưu dữ liệu giống vậy để dễ quản lý</t>
   </si>
 </sst>
 </file>
@@ -621,6 +618,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -638,12 +641,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -961,8 +958,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B71D19A7-44BD-47E8-BCBA-FDF3CC1D1199}">
   <dimension ref="C1:K94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D67" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="K85" sqref="K85"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H83" sqref="H83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -977,13 +974,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G1" s="12" t="s">
+      <c r="G1" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
-      <c r="J1" s="12"/>
-      <c r="K1" s="12"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14"/>
     </row>
     <row r="2" spans="7:11" x14ac:dyDescent="0.25">
       <c r="G2" s="1" t="s">
@@ -1033,7 +1030,7 @@
         <v>18</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="7:11" x14ac:dyDescent="0.25">
@@ -1041,7 +1038,7 @@
         <v>3</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="I5" s="2" t="s">
         <v>17</v>
@@ -1054,13 +1051,13 @@
       </c>
     </row>
     <row r="7" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G7" s="12" t="s">
+      <c r="G7" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="H7" s="12"/>
-      <c r="I7" s="12"/>
-      <c r="J7" s="12"/>
-      <c r="K7" s="12"/>
+      <c r="H7" s="14"/>
+      <c r="I7" s="14"/>
+      <c r="J7" s="14"/>
+      <c r="K7" s="14"/>
     </row>
     <row r="8" spans="7:11" x14ac:dyDescent="0.25">
       <c r="G8" s="1" t="s">
@@ -1118,7 +1115,7 @@
         <v>3</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="I11" s="2" t="s">
         <v>17</v>
@@ -1131,13 +1128,13 @@
       </c>
     </row>
     <row r="13" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G13" s="12" t="s">
+      <c r="G13" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="H13" s="12"/>
-      <c r="I13" s="12"/>
-      <c r="J13" s="12"/>
-      <c r="K13" s="12"/>
+      <c r="H13" s="14"/>
+      <c r="I13" s="14"/>
+      <c r="J13" s="14"/>
+      <c r="K13" s="14"/>
     </row>
     <row r="14" spans="7:11" x14ac:dyDescent="0.25">
       <c r="G14" s="1" t="s">
@@ -1187,7 +1184,7 @@
         <v>18</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="17" spans="7:11" x14ac:dyDescent="0.25">
@@ -1195,7 +1192,7 @@
         <v>3</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="I17" s="2" t="s">
         <v>17</v>
@@ -1208,13 +1205,13 @@
       </c>
     </row>
     <row r="19" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G19" s="12" t="s">
+      <c r="G19" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="H19" s="12"/>
-      <c r="I19" s="12"/>
-      <c r="J19" s="12"/>
-      <c r="K19" s="12"/>
+      <c r="H19" s="14"/>
+      <c r="I19" s="14"/>
+      <c r="J19" s="14"/>
+      <c r="K19" s="14"/>
     </row>
     <row r="20" spans="7:11" x14ac:dyDescent="0.25">
       <c r="G20" s="1" t="s">
@@ -1264,7 +1261,7 @@
         <v>18</v>
       </c>
       <c r="K22" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="23" spans="7:11" x14ac:dyDescent="0.25">
@@ -1281,7 +1278,7 @@
         <v>12</v>
       </c>
       <c r="K23" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="24" spans="7:11" x14ac:dyDescent="0.25">
@@ -1289,7 +1286,7 @@
         <v>4</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="I24" s="2" t="s">
         <v>15</v>
@@ -1306,7 +1303,7 @@
         <v>5</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="I25" s="2" t="s">
         <v>15</v>
@@ -1323,7 +1320,7 @@
         <v>6</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="I26" s="2" t="s">
         <v>15</v>
@@ -1340,7 +1337,7 @@
         <v>7</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="I27" s="2" t="s">
         <v>6</v>
@@ -1349,7 +1346,7 @@
         <v>35</v>
       </c>
       <c r="K27" s="2" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="28" spans="7:11" x14ac:dyDescent="0.25">
@@ -1383,7 +1380,7 @@
         <v>12</v>
       </c>
       <c r="K29" s="2" t="s">
-        <v>40</v>
+        <v>123</v>
       </c>
     </row>
     <row r="30" spans="7:11" x14ac:dyDescent="0.25">
@@ -1400,7 +1397,7 @@
         <v>37</v>
       </c>
       <c r="K30" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="31" spans="7:11" x14ac:dyDescent="0.25">
@@ -1408,7 +1405,7 @@
         <v>11</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="I31" s="2" t="s">
         <v>17</v>
@@ -1421,25 +1418,25 @@
       </c>
     </row>
     <row r="33" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C33" s="19" t="s">
-        <v>126</v>
-      </c>
-      <c r="D33" s="18"/>
-      <c r="E33" s="18"/>
-      <c r="F33" s="18"/>
-      <c r="G33" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="H33" s="12"/>
-      <c r="I33" s="12"/>
-      <c r="J33" s="12"/>
-      <c r="K33" s="12"/>
+      <c r="C33" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="D33" s="13"/>
+      <c r="E33" s="13"/>
+      <c r="F33" s="13"/>
+      <c r="G33" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="H33" s="14"/>
+      <c r="I33" s="14"/>
+      <c r="J33" s="14"/>
+      <c r="K33" s="14"/>
     </row>
     <row r="34" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C34" s="18"/>
-      <c r="D34" s="18"/>
-      <c r="E34" s="18"/>
-      <c r="F34" s="18"/>
+      <c r="C34" s="13"/>
+      <c r="D34" s="13"/>
+      <c r="E34" s="13"/>
+      <c r="F34" s="13"/>
       <c r="G34" s="1" t="s">
         <v>1</v>
       </c>
@@ -1457,10 +1454,10 @@
       </c>
     </row>
     <row r="35" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C35" s="18"/>
-      <c r="D35" s="18"/>
-      <c r="E35" s="18"/>
-      <c r="F35" s="18"/>
+      <c r="C35" s="13"/>
+      <c r="D35" s="13"/>
+      <c r="E35" s="13"/>
+      <c r="F35" s="13"/>
       <c r="G35" s="2">
         <v>1</v>
       </c>
@@ -1478,120 +1475,120 @@
       </c>
     </row>
     <row r="36" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C36" s="18"/>
-      <c r="D36" s="18"/>
-      <c r="E36" s="18"/>
-      <c r="F36" s="18"/>
+      <c r="C36" s="13"/>
+      <c r="D36" s="13"/>
+      <c r="E36" s="13"/>
+      <c r="F36" s="13"/>
       <c r="G36" s="2">
         <v>2</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="I36" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J36" s="2" t="s">
         <v>12</v>
       </c>
       <c r="K36" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="37" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C37" s="18"/>
-      <c r="D37" s="18"/>
-      <c r="E37" s="18"/>
-      <c r="F37" s="18"/>
+      <c r="C37" s="13"/>
+      <c r="D37" s="13"/>
+      <c r="E37" s="13"/>
+      <c r="F37" s="13"/>
       <c r="G37" s="2">
         <v>3</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="I37" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J37" s="2" t="s">
         <v>12</v>
       </c>
       <c r="K37" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="38" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C38" s="18"/>
-      <c r="D38" s="18"/>
-      <c r="E38" s="18"/>
-      <c r="F38" s="18"/>
+      <c r="C38" s="13"/>
+      <c r="D38" s="13"/>
+      <c r="E38" s="13"/>
+      <c r="F38" s="13"/>
       <c r="G38" s="2">
         <v>4</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="I38" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J38" s="2" t="s">
         <v>12</v>
       </c>
       <c r="K38" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="39" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C39" s="18"/>
-      <c r="D39" s="18"/>
-      <c r="E39" s="18"/>
-      <c r="F39" s="18"/>
+      <c r="C39" s="13"/>
+      <c r="D39" s="13"/>
+      <c r="E39" s="13"/>
+      <c r="F39" s="13"/>
       <c r="G39" s="2">
         <v>5</v>
       </c>
       <c r="H39" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I39" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J39" s="2" t="s">
         <v>12</v>
       </c>
       <c r="K39" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="40" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C40" s="18"/>
-      <c r="D40" s="18"/>
-      <c r="E40" s="18"/>
-      <c r="F40" s="18"/>
+      <c r="C40" s="13"/>
+      <c r="D40" s="13"/>
+      <c r="E40" s="13"/>
+      <c r="F40" s="13"/>
       <c r="G40" s="2">
         <v>6</v>
       </c>
       <c r="H40" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I40" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="J40" s="2" t="s">
         <v>18</v>
       </c>
       <c r="K40" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="41" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C41" s="18"/>
-      <c r="D41" s="18"/>
-      <c r="E41" s="18"/>
-      <c r="F41" s="18"/>
+      <c r="C41" s="13"/>
+      <c r="D41" s="13"/>
+      <c r="E41" s="13"/>
+      <c r="F41" s="13"/>
       <c r="G41" s="2">
         <v>7</v>
       </c>
       <c r="H41" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I41" s="2" t="s">
         <v>17</v>
@@ -1600,59 +1597,59 @@
         <v>19</v>
       </c>
       <c r="K41" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="42" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C42" s="18"/>
-      <c r="D42" s="18"/>
-      <c r="E42" s="18"/>
-      <c r="F42" s="18"/>
+      <c r="C42" s="13"/>
+      <c r="D42" s="13"/>
+      <c r="E42" s="13"/>
+      <c r="F42" s="13"/>
       <c r="G42" s="2">
         <v>8</v>
       </c>
       <c r="H42" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I42" s="2" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="J42" s="2" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="K42" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="43" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C43" s="18"/>
-      <c r="D43" s="18"/>
-      <c r="E43" s="18"/>
-      <c r="F43" s="18"/>
+      <c r="C43" s="13"/>
+      <c r="D43" s="13"/>
+      <c r="E43" s="13"/>
+      <c r="F43" s="13"/>
       <c r="G43" s="2">
         <v>9</v>
       </c>
       <c r="H43" s="2" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="I43" s="2" t="s">
         <v>32</v>
       </c>
       <c r="J43" s="2"/>
       <c r="K43" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="44" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C44" s="18"/>
-      <c r="D44" s="18"/>
-      <c r="E44" s="18"/>
-      <c r="F44" s="18"/>
+      <c r="C44" s="13"/>
+      <c r="D44" s="13"/>
+      <c r="E44" s="13"/>
+      <c r="F44" s="13"/>
       <c r="G44" s="2">
         <v>10</v>
       </c>
       <c r="H44" s="2" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="I44" s="2" t="s">
         <v>17</v>
@@ -1661,19 +1658,19 @@
         <v>19</v>
       </c>
       <c r="K44" s="2" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="45" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C45" s="18"/>
-      <c r="D45" s="18"/>
-      <c r="E45" s="18"/>
-      <c r="F45" s="18"/>
+      <c r="C45" s="13"/>
+      <c r="D45" s="13"/>
+      <c r="E45" s="13"/>
+      <c r="F45" s="13"/>
       <c r="G45" s="2">
         <v>11</v>
       </c>
       <c r="H45" s="2" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="I45" s="2" t="s">
         <v>17</v>
@@ -1693,13 +1690,13 @@
       <c r="K46" s="11"/>
     </row>
     <row r="47" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="G47" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="H47" s="12"/>
-      <c r="I47" s="12"/>
-      <c r="J47" s="12"/>
-      <c r="K47" s="12"/>
+      <c r="G47" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="H47" s="14"/>
+      <c r="I47" s="14"/>
+      <c r="J47" s="14"/>
+      <c r="K47" s="14"/>
     </row>
     <row r="48" spans="3:11" x14ac:dyDescent="0.25">
       <c r="G48" s="1" t="s">
@@ -1740,16 +1737,16 @@
         <v>2</v>
       </c>
       <c r="H50" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="I50" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J50" s="2" t="s">
         <v>12</v>
       </c>
       <c r="K50" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="51" spans="7:11" x14ac:dyDescent="0.25">
@@ -1757,16 +1754,16 @@
         <v>3</v>
       </c>
       <c r="H51" s="2" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="I51" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J51" s="2" t="s">
         <v>12</v>
       </c>
       <c r="K51" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="52" spans="7:11" x14ac:dyDescent="0.25">
@@ -1774,16 +1771,16 @@
         <v>4</v>
       </c>
       <c r="H52" s="2" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="I52" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J52" s="2" t="s">
         <v>12</v>
       </c>
       <c r="K52" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="53" spans="7:11" x14ac:dyDescent="0.25">
@@ -1791,16 +1788,16 @@
         <v>5</v>
       </c>
       <c r="H53" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I53" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J53" s="2" t="s">
         <v>12</v>
       </c>
       <c r="K53" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="54" spans="7:11" x14ac:dyDescent="0.25">
@@ -1808,16 +1805,16 @@
         <v>6</v>
       </c>
       <c r="H54" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I54" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="J54" s="2" t="s">
         <v>18</v>
       </c>
       <c r="K54" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="55" spans="7:11" x14ac:dyDescent="0.25">
@@ -1825,16 +1822,16 @@
         <v>7</v>
       </c>
       <c r="H55" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I55" s="2" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="J55" s="2" t="s">
         <v>18</v>
       </c>
       <c r="K55" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="56" spans="7:11" x14ac:dyDescent="0.25">
@@ -1842,16 +1839,16 @@
         <v>8</v>
       </c>
       <c r="H56" s="2" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="I56" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J56" s="2" t="s">
         <v>18</v>
       </c>
       <c r="K56" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="57" spans="7:11" x14ac:dyDescent="0.25">
@@ -1859,7 +1856,7 @@
         <v>9</v>
       </c>
       <c r="H57" s="2" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="I57" s="2" t="s">
         <v>32</v>
@@ -1868,7 +1865,7 @@
         <v>12</v>
       </c>
       <c r="K57" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="58" spans="7:11" x14ac:dyDescent="0.25">
@@ -1876,7 +1873,7 @@
         <v>10</v>
       </c>
       <c r="H58" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I58" s="2" t="s">
         <v>17</v>
@@ -1885,7 +1882,7 @@
         <v>19</v>
       </c>
       <c r="K58" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="59" spans="7:11" x14ac:dyDescent="0.25">
@@ -1893,7 +1890,7 @@
         <v>11</v>
       </c>
       <c r="H59" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I59" s="2" t="s">
         <v>17</v>
@@ -1902,7 +1899,7 @@
         <v>19</v>
       </c>
       <c r="K59" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="60" spans="7:11" x14ac:dyDescent="0.25">
@@ -1910,7 +1907,7 @@
         <v>12</v>
       </c>
       <c r="H60" s="2" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="I60" s="2" t="s">
         <v>17</v>
@@ -1919,7 +1916,7 @@
         <v>19</v>
       </c>
       <c r="K60" s="2" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="61" spans="7:11" x14ac:dyDescent="0.25">
@@ -1927,7 +1924,7 @@
         <v>13</v>
       </c>
       <c r="H61" s="2" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="I61" s="2" t="s">
         <v>17</v>
@@ -1940,13 +1937,13 @@
       </c>
     </row>
     <row r="63" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G63" s="12" t="s">
-        <v>92</v>
-      </c>
-      <c r="H63" s="12"/>
-      <c r="I63" s="12"/>
-      <c r="J63" s="12"/>
-      <c r="K63" s="12"/>
+      <c r="G63" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="H63" s="14"/>
+      <c r="I63" s="14"/>
+      <c r="J63" s="14"/>
+      <c r="K63" s="14"/>
     </row>
     <row r="64" spans="7:11" x14ac:dyDescent="0.25">
       <c r="G64" s="1" t="s">
@@ -2004,16 +2001,16 @@
         <v>3</v>
       </c>
       <c r="H67" s="2" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="I67" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J67" s="10" t="s">
         <v>12</v>
       </c>
       <c r="K67" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="68" spans="7:11" x14ac:dyDescent="0.25">
@@ -2021,16 +2018,16 @@
         <v>4</v>
       </c>
       <c r="H68" s="2" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="I68" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J68" s="10" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="K68" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="69" spans="7:11" x14ac:dyDescent="0.25">
@@ -2038,7 +2035,7 @@
         <v>5</v>
       </c>
       <c r="H69" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I69" s="10" t="s">
         <v>31</v>
@@ -2047,7 +2044,7 @@
         <v>36</v>
       </c>
       <c r="K69" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="70" spans="7:11" x14ac:dyDescent="0.25">
@@ -2055,16 +2052,16 @@
         <v>6</v>
       </c>
       <c r="H70" s="2" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="I70" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="J70" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="J70" s="10" t="s">
-        <v>69</v>
-      </c>
       <c r="K70" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="71" spans="7:11" x14ac:dyDescent="0.25">
@@ -2081,7 +2078,7 @@
         <v>37</v>
       </c>
       <c r="K71" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="72" spans="7:11" x14ac:dyDescent="0.25">
@@ -2089,7 +2086,7 @@
         <v>8</v>
       </c>
       <c r="H72" s="2" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="I72" s="2" t="s">
         <v>17</v>
@@ -2102,13 +2099,13 @@
       </c>
     </row>
     <row r="74" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G74" s="13" t="s">
-        <v>93</v>
-      </c>
-      <c r="H74" s="14"/>
-      <c r="I74" s="14"/>
-      <c r="J74" s="14"/>
-      <c r="K74" s="15"/>
+      <c r="G74" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="H74" s="16"/>
+      <c r="I74" s="16"/>
+      <c r="J74" s="16"/>
+      <c r="K74" s="17"/>
     </row>
     <row r="75" spans="7:11" x14ac:dyDescent="0.25">
       <c r="G75" s="4" t="s">
@@ -2149,16 +2146,16 @@
         <v>2</v>
       </c>
       <c r="H77" s="2" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="I77" s="8" t="s">
         <v>15</v>
       </c>
       <c r="J77" s="2" t="s">
-        <v>34</v>
+        <v>93</v>
       </c>
       <c r="K77" s="8" t="s">
-        <v>81</v>
+        <v>124</v>
       </c>
     </row>
     <row r="78" spans="7:11" x14ac:dyDescent="0.25">
@@ -2166,7 +2163,7 @@
         <v>3</v>
       </c>
       <c r="H78" s="2" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="I78" s="8" t="s">
         <v>15</v>
@@ -2175,7 +2172,7 @@
         <v>34</v>
       </c>
       <c r="K78" s="8" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="79" spans="7:11" x14ac:dyDescent="0.25">
@@ -2183,16 +2180,16 @@
         <v>4</v>
       </c>
       <c r="H79" s="2" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="I79" s="8" t="s">
         <v>15</v>
       </c>
       <c r="J79" s="2" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="K79" s="8" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="80" spans="7:11" x14ac:dyDescent="0.25">
@@ -2200,16 +2197,16 @@
         <v>5</v>
       </c>
       <c r="H80" s="2" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="I80" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J80" s="8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K80" s="8" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="81" spans="7:11" x14ac:dyDescent="0.25">
@@ -2217,16 +2214,16 @@
         <v>6</v>
       </c>
       <c r="H81" s="2" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="I81" s="10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J81" s="8" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="K81" s="8" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="82" spans="7:11" x14ac:dyDescent="0.25">
@@ -2234,16 +2231,16 @@
         <v>7</v>
       </c>
       <c r="H82" s="2" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="I82" s="10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J82" s="8" t="s">
         <v>12</v>
       </c>
       <c r="K82" s="8" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="83" spans="7:11" x14ac:dyDescent="0.25">
@@ -2251,16 +2248,16 @@
         <v>8</v>
       </c>
       <c r="H83" s="2" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="I83" s="10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J83" s="8" t="s">
         <v>12</v>
       </c>
       <c r="K83" s="8" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="84" spans="7:11" x14ac:dyDescent="0.25">
@@ -2268,16 +2265,16 @@
         <v>9</v>
       </c>
       <c r="H84" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I84" s="10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J84" s="8" t="s">
-        <v>86</v>
+        <v>12</v>
       </c>
       <c r="K84" s="8" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="85" spans="7:11" x14ac:dyDescent="0.25">
@@ -2285,14 +2282,14 @@
         <v>10</v>
       </c>
       <c r="H85" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="I85" s="10" t="s">
         <v>77</v>
-      </c>
-      <c r="I85" s="10" t="s">
-        <v>78</v>
       </c>
       <c r="J85" s="8"/>
       <c r="K85" s="8" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
     <row r="86" spans="7:11" x14ac:dyDescent="0.25">
@@ -2300,7 +2297,7 @@
         <v>11</v>
       </c>
       <c r="H86" s="2" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="I86" s="8" t="s">
         <v>17</v>
@@ -2313,13 +2310,13 @@
       </c>
     </row>
     <row r="88" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G88" s="13" t="s">
-        <v>94</v>
-      </c>
-      <c r="H88" s="14"/>
-      <c r="I88" s="14"/>
-      <c r="J88" s="14"/>
-      <c r="K88" s="15"/>
+      <c r="G88" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="H88" s="16"/>
+      <c r="I88" s="16"/>
+      <c r="J88" s="16"/>
+      <c r="K88" s="17"/>
     </row>
     <row r="89" spans="7:11" x14ac:dyDescent="0.25">
       <c r="G89" s="4" t="s">
@@ -2343,16 +2340,16 @@
         <v>1</v>
       </c>
       <c r="H90" s="7" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="I90" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="J90" s="16" t="s">
-        <v>87</v>
+      <c r="J90" s="18" t="s">
+        <v>84</v>
       </c>
       <c r="K90" s="8" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="91" spans="7:11" x14ac:dyDescent="0.25">
@@ -2360,14 +2357,14 @@
         <v>2</v>
       </c>
       <c r="H91" s="7" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="I91" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="J91" s="17"/>
+      <c r="J91" s="19"/>
       <c r="K91" s="8" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="92" spans="7:11" x14ac:dyDescent="0.25">
@@ -2381,10 +2378,10 @@
         <v>6</v>
       </c>
       <c r="J92" s="10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="K92" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="93" spans="7:11" x14ac:dyDescent="0.25">
@@ -2401,7 +2398,7 @@
         <v>36</v>
       </c>
       <c r="K93" s="8" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="94" spans="7:11" x14ac:dyDescent="0.25">
@@ -2409,7 +2406,7 @@
         <v>5</v>
       </c>
       <c r="H94" s="8" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="I94" s="8" t="s">
         <v>17</v>
@@ -2423,17 +2420,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="C33:F45"/>
-    <mergeCell ref="G47:K47"/>
-    <mergeCell ref="G63:K63"/>
-    <mergeCell ref="G74:K74"/>
-    <mergeCell ref="G88:K88"/>
     <mergeCell ref="J90:J91"/>
     <mergeCell ref="G33:K33"/>
     <mergeCell ref="G1:K1"/>
     <mergeCell ref="G7:K7"/>
     <mergeCell ref="G13:K13"/>
     <mergeCell ref="G19:K19"/>
+    <mergeCell ref="C33:F45"/>
+    <mergeCell ref="G47:K47"/>
+    <mergeCell ref="G63:K63"/>
+    <mergeCell ref="G74:K74"/>
+    <mergeCell ref="G88:K88"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Generate script using SQL Server
</commit_message>
<xml_diff>
--- a/database/Database-In-More-Detail.xlsx
+++ b/database/Database-In-More-Detail.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\Book-Shop-API\database\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\BookShop-API\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5092BAC2-8D74-4914-A2E6-2133F8539C1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC15EEB9-73F3-4025-86BB-8B0E7BE345BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{DBAE516F-9EAD-4516-8555-9494F8FA5157}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{DBAE516F-9EAD-4516-8555-9494F8FA5157}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="129">
   <si>
     <t>Publisher</t>
   </si>
@@ -422,6 +422,9 @@
   </si>
   <si>
     <t>Trạng thái hóa đơn ("Thành công", "Đang vận chuyển", "Lỗi",…) lưu dữ liệu giống vậy để dễ quản lý</t>
+  </si>
+  <si>
+    <t>varchar(max)</t>
   </si>
 </sst>
 </file>
@@ -618,13 +621,19 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -634,12 +643,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -958,8 +961,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B71D19A7-44BD-47E8-BCBA-FDF3CC1D1199}">
   <dimension ref="C1:K94"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H83" sqref="H83"/>
+    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="J69" sqref="J69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1374,11 +1377,9 @@
         <v>30</v>
       </c>
       <c r="I29" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="J29" s="2" t="s">
-        <v>12</v>
-      </c>
+        <v>128</v>
+      </c>
+      <c r="J29" s="2"/>
       <c r="K29" s="2" t="s">
         <v>123</v>
       </c>
@@ -1418,12 +1419,12 @@
       </c>
     </row>
     <row r="33" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C33" s="12" t="s">
+      <c r="C33" s="15" t="s">
         <v>122</v>
       </c>
-      <c r="D33" s="13"/>
-      <c r="E33" s="13"/>
-      <c r="F33" s="13"/>
+      <c r="D33" s="16"/>
+      <c r="E33" s="16"/>
+      <c r="F33" s="16"/>
       <c r="G33" s="14" t="s">
         <v>43</v>
       </c>
@@ -1433,10 +1434,10 @@
       <c r="K33" s="14"/>
     </row>
     <row r="34" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C34" s="13"/>
-      <c r="D34" s="13"/>
-      <c r="E34" s="13"/>
-      <c r="F34" s="13"/>
+      <c r="C34" s="16"/>
+      <c r="D34" s="16"/>
+      <c r="E34" s="16"/>
+      <c r="F34" s="16"/>
       <c r="G34" s="1" t="s">
         <v>1</v>
       </c>
@@ -1454,10 +1455,10 @@
       </c>
     </row>
     <row r="35" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C35" s="13"/>
-      <c r="D35" s="13"/>
-      <c r="E35" s="13"/>
-      <c r="F35" s="13"/>
+      <c r="C35" s="16"/>
+      <c r="D35" s="16"/>
+      <c r="E35" s="16"/>
+      <c r="F35" s="16"/>
       <c r="G35" s="2">
         <v>1</v>
       </c>
@@ -1475,10 +1476,10 @@
       </c>
     </row>
     <row r="36" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C36" s="13"/>
-      <c r="D36" s="13"/>
-      <c r="E36" s="13"/>
-      <c r="F36" s="13"/>
+      <c r="C36" s="16"/>
+      <c r="D36" s="16"/>
+      <c r="E36" s="16"/>
+      <c r="F36" s="16"/>
       <c r="G36" s="2">
         <v>2</v>
       </c>
@@ -1496,10 +1497,10 @@
       </c>
     </row>
     <row r="37" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C37" s="13"/>
-      <c r="D37" s="13"/>
-      <c r="E37" s="13"/>
-      <c r="F37" s="13"/>
+      <c r="C37" s="16"/>
+      <c r="D37" s="16"/>
+      <c r="E37" s="16"/>
+      <c r="F37" s="16"/>
       <c r="G37" s="2">
         <v>3</v>
       </c>
@@ -1517,10 +1518,10 @@
       </c>
     </row>
     <row r="38" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C38" s="13"/>
-      <c r="D38" s="13"/>
-      <c r="E38" s="13"/>
-      <c r="F38" s="13"/>
+      <c r="C38" s="16"/>
+      <c r="D38" s="16"/>
+      <c r="E38" s="16"/>
+      <c r="F38" s="16"/>
       <c r="G38" s="2">
         <v>4</v>
       </c>
@@ -1538,10 +1539,10 @@
       </c>
     </row>
     <row r="39" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C39" s="13"/>
-      <c r="D39" s="13"/>
-      <c r="E39" s="13"/>
-      <c r="F39" s="13"/>
+      <c r="C39" s="16"/>
+      <c r="D39" s="16"/>
+      <c r="E39" s="16"/>
+      <c r="F39" s="16"/>
       <c r="G39" s="2">
         <v>5</v>
       </c>
@@ -1559,10 +1560,10 @@
       </c>
     </row>
     <row r="40" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C40" s="13"/>
-      <c r="D40" s="13"/>
-      <c r="E40" s="13"/>
-      <c r="F40" s="13"/>
+      <c r="C40" s="16"/>
+      <c r="D40" s="16"/>
+      <c r="E40" s="16"/>
+      <c r="F40" s="16"/>
       <c r="G40" s="2">
         <v>6</v>
       </c>
@@ -1580,10 +1581,10 @@
       </c>
     </row>
     <row r="41" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C41" s="13"/>
-      <c r="D41" s="13"/>
-      <c r="E41" s="13"/>
-      <c r="F41" s="13"/>
+      <c r="C41" s="16"/>
+      <c r="D41" s="16"/>
+      <c r="E41" s="16"/>
+      <c r="F41" s="16"/>
       <c r="G41" s="2">
         <v>7</v>
       </c>
@@ -1601,10 +1602,10 @@
       </c>
     </row>
     <row r="42" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C42" s="13"/>
-      <c r="D42" s="13"/>
-      <c r="E42" s="13"/>
-      <c r="F42" s="13"/>
+      <c r="C42" s="16"/>
+      <c r="D42" s="16"/>
+      <c r="E42" s="16"/>
+      <c r="F42" s="16"/>
       <c r="G42" s="2">
         <v>8</v>
       </c>
@@ -1622,10 +1623,10 @@
       </c>
     </row>
     <row r="43" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C43" s="13"/>
-      <c r="D43" s="13"/>
-      <c r="E43" s="13"/>
-      <c r="F43" s="13"/>
+      <c r="C43" s="16"/>
+      <c r="D43" s="16"/>
+      <c r="E43" s="16"/>
+      <c r="F43" s="16"/>
       <c r="G43" s="2">
         <v>9</v>
       </c>
@@ -1641,10 +1642,10 @@
       </c>
     </row>
     <row r="44" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C44" s="13"/>
-      <c r="D44" s="13"/>
-      <c r="E44" s="13"/>
-      <c r="F44" s="13"/>
+      <c r="C44" s="16"/>
+      <c r="D44" s="16"/>
+      <c r="E44" s="16"/>
+      <c r="F44" s="16"/>
       <c r="G44" s="2">
         <v>10</v>
       </c>
@@ -1662,10 +1663,10 @@
       </c>
     </row>
     <row r="45" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C45" s="13"/>
-      <c r="D45" s="13"/>
-      <c r="E45" s="13"/>
-      <c r="F45" s="13"/>
+      <c r="C45" s="16"/>
+      <c r="D45" s="16"/>
+      <c r="E45" s="16"/>
+      <c r="F45" s="16"/>
       <c r="G45" s="2">
         <v>11</v>
       </c>
@@ -2099,13 +2100,13 @@
       </c>
     </row>
     <row r="74" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G74" s="15" t="s">
+      <c r="G74" s="17" t="s">
         <v>90</v>
       </c>
-      <c r="H74" s="16"/>
-      <c r="I74" s="16"/>
-      <c r="J74" s="16"/>
-      <c r="K74" s="17"/>
+      <c r="H74" s="18"/>
+      <c r="I74" s="18"/>
+      <c r="J74" s="18"/>
+      <c r="K74" s="19"/>
     </row>
     <row r="75" spans="7:11" x14ac:dyDescent="0.25">
       <c r="G75" s="4" t="s">
@@ -2310,13 +2311,13 @@
       </c>
     </row>
     <row r="88" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G88" s="15" t="s">
+      <c r="G88" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="H88" s="16"/>
-      <c r="I88" s="16"/>
-      <c r="J88" s="16"/>
-      <c r="K88" s="17"/>
+      <c r="H88" s="18"/>
+      <c r="I88" s="18"/>
+      <c r="J88" s="18"/>
+      <c r="K88" s="19"/>
     </row>
     <row r="89" spans="7:11" x14ac:dyDescent="0.25">
       <c r="G89" s="4" t="s">
@@ -2345,7 +2346,7 @@
       <c r="I90" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="J90" s="18" t="s">
+      <c r="J90" s="12" t="s">
         <v>84</v>
       </c>
       <c r="K90" s="8" t="s">
@@ -2362,7 +2363,7 @@
       <c r="I91" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="J91" s="19"/>
+      <c r="J91" s="13"/>
       <c r="K91" s="8" t="s">
         <v>86</v>
       </c>
@@ -2420,17 +2421,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="C33:F45"/>
+    <mergeCell ref="G47:K47"/>
+    <mergeCell ref="G63:K63"/>
+    <mergeCell ref="G74:K74"/>
+    <mergeCell ref="G88:K88"/>
     <mergeCell ref="J90:J91"/>
     <mergeCell ref="G33:K33"/>
     <mergeCell ref="G1:K1"/>
     <mergeCell ref="G7:K7"/>
     <mergeCell ref="G13:K13"/>
     <mergeCell ref="G19:K19"/>
-    <mergeCell ref="C33:F45"/>
-    <mergeCell ref="G47:K47"/>
-    <mergeCell ref="G63:K63"/>
-    <mergeCell ref="G74:K74"/>
-    <mergeCell ref="G88:K88"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Add AuditLog into excel
</commit_message>
<xml_diff>
--- a/database/Database-In-More-Detail.xlsx
+++ b/database/Database-In-More-Detail.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\BookShop-API\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC15EEB9-73F3-4025-86BB-8B0E7BE345BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B189765-D708-4B98-9843-7FCFA6CAE2F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{DBAE516F-9EAD-4516-8555-9494F8FA5157}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{DBAE516F-9EAD-4516-8555-9494F8FA5157}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="149">
   <si>
     <t>Publisher</t>
   </si>
@@ -425,6 +425,66 @@
   </si>
   <si>
     <t>varchar(max)</t>
+  </si>
+  <si>
+    <t>AuditLog</t>
+  </si>
+  <si>
+    <t>Mã nhân viên</t>
+  </si>
+  <si>
+    <t>action</t>
+  </si>
+  <si>
+    <t>entityName</t>
+  </si>
+  <si>
+    <t>entityId</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>timestamp</t>
+  </si>
+  <si>
+    <t>ipAddress</t>
+  </si>
+  <si>
+    <t>userAgent</t>
+  </si>
+  <si>
+    <t>nvarchar(max)</t>
+  </si>
+  <si>
+    <t>datetime2(7)</t>
+  </si>
+  <si>
+    <t>nvarchar(54)</t>
+  </si>
+  <si>
+    <t>nvarchar(200)</t>
+  </si>
+  <si>
+    <t>Hành động</t>
+  </si>
+  <si>
+    <t>Tên bảng</t>
+  </si>
+  <si>
+    <t>Id của đối tượng</t>
+  </si>
+  <si>
+    <t>Mô tả</t>
+  </si>
+  <si>
+    <t>Thời gian</t>
+  </si>
+  <si>
+    <t>Địa chỉ ip</t>
+  </si>
+  <si>
+    <t>Tác nhân người dùng</t>
   </si>
 </sst>
 </file>
@@ -586,7 +646,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -621,19 +681,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -644,6 +698,15 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -959,10 +1022,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B71D19A7-44BD-47E8-BCBA-FDF3CC1D1199}">
-  <dimension ref="C1:K94"/>
+  <dimension ref="C1:K106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="J69" sqref="J69"/>
+    <sheetView tabSelected="1" topLeftCell="A79" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K109" sqref="K109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1419,12 +1482,12 @@
       </c>
     </row>
     <row r="33" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C33" s="15" t="s">
+      <c r="C33" s="12" t="s">
         <v>122</v>
       </c>
-      <c r="D33" s="16"/>
-      <c r="E33" s="16"/>
-      <c r="F33" s="16"/>
+      <c r="D33" s="13"/>
+      <c r="E33" s="13"/>
+      <c r="F33" s="13"/>
       <c r="G33" s="14" t="s">
         <v>43</v>
       </c>
@@ -1434,10 +1497,10 @@
       <c r="K33" s="14"/>
     </row>
     <row r="34" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C34" s="16"/>
-      <c r="D34" s="16"/>
-      <c r="E34" s="16"/>
-      <c r="F34" s="16"/>
+      <c r="C34" s="13"/>
+      <c r="D34" s="13"/>
+      <c r="E34" s="13"/>
+      <c r="F34" s="13"/>
       <c r="G34" s="1" t="s">
         <v>1</v>
       </c>
@@ -1455,10 +1518,10 @@
       </c>
     </row>
     <row r="35" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C35" s="16"/>
-      <c r="D35" s="16"/>
-      <c r="E35" s="16"/>
-      <c r="F35" s="16"/>
+      <c r="C35" s="13"/>
+      <c r="D35" s="13"/>
+      <c r="E35" s="13"/>
+      <c r="F35" s="13"/>
       <c r="G35" s="2">
         <v>1</v>
       </c>
@@ -1476,10 +1539,10 @@
       </c>
     </row>
     <row r="36" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C36" s="16"/>
-      <c r="D36" s="16"/>
-      <c r="E36" s="16"/>
-      <c r="F36" s="16"/>
+      <c r="C36" s="13"/>
+      <c r="D36" s="13"/>
+      <c r="E36" s="13"/>
+      <c r="F36" s="13"/>
       <c r="G36" s="2">
         <v>2</v>
       </c>
@@ -1497,10 +1560,10 @@
       </c>
     </row>
     <row r="37" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C37" s="16"/>
-      <c r="D37" s="16"/>
-      <c r="E37" s="16"/>
-      <c r="F37" s="16"/>
+      <c r="C37" s="13"/>
+      <c r="D37" s="13"/>
+      <c r="E37" s="13"/>
+      <c r="F37" s="13"/>
       <c r="G37" s="2">
         <v>3</v>
       </c>
@@ -1518,10 +1581,10 @@
       </c>
     </row>
     <row r="38" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C38" s="16"/>
-      <c r="D38" s="16"/>
-      <c r="E38" s="16"/>
-      <c r="F38" s="16"/>
+      <c r="C38" s="13"/>
+      <c r="D38" s="13"/>
+      <c r="E38" s="13"/>
+      <c r="F38" s="13"/>
       <c r="G38" s="2">
         <v>4</v>
       </c>
@@ -1539,10 +1602,10 @@
       </c>
     </row>
     <row r="39" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C39" s="16"/>
-      <c r="D39" s="16"/>
-      <c r="E39" s="16"/>
-      <c r="F39" s="16"/>
+      <c r="C39" s="13"/>
+      <c r="D39" s="13"/>
+      <c r="E39" s="13"/>
+      <c r="F39" s="13"/>
       <c r="G39" s="2">
         <v>5</v>
       </c>
@@ -1560,10 +1623,10 @@
       </c>
     </row>
     <row r="40" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C40" s="16"/>
-      <c r="D40" s="16"/>
-      <c r="E40" s="16"/>
-      <c r="F40" s="16"/>
+      <c r="C40" s="13"/>
+      <c r="D40" s="13"/>
+      <c r="E40" s="13"/>
+      <c r="F40" s="13"/>
       <c r="G40" s="2">
         <v>6</v>
       </c>
@@ -1581,10 +1644,10 @@
       </c>
     </row>
     <row r="41" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C41" s="16"/>
-      <c r="D41" s="16"/>
-      <c r="E41" s="16"/>
-      <c r="F41" s="16"/>
+      <c r="C41" s="13"/>
+      <c r="D41" s="13"/>
+      <c r="E41" s="13"/>
+      <c r="F41" s="13"/>
       <c r="G41" s="2">
         <v>7</v>
       </c>
@@ -1602,10 +1665,10 @@
       </c>
     </row>
     <row r="42" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C42" s="16"/>
-      <c r="D42" s="16"/>
-      <c r="E42" s="16"/>
-      <c r="F42" s="16"/>
+      <c r="C42" s="13"/>
+      <c r="D42" s="13"/>
+      <c r="E42" s="13"/>
+      <c r="F42" s="13"/>
       <c r="G42" s="2">
         <v>8</v>
       </c>
@@ -1623,10 +1686,10 @@
       </c>
     </row>
     <row r="43" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C43" s="16"/>
-      <c r="D43" s="16"/>
-      <c r="E43" s="16"/>
-      <c r="F43" s="16"/>
+      <c r="C43" s="13"/>
+      <c r="D43" s="13"/>
+      <c r="E43" s="13"/>
+      <c r="F43" s="13"/>
       <c r="G43" s="2">
         <v>9</v>
       </c>
@@ -1642,10 +1705,10 @@
       </c>
     </row>
     <row r="44" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C44" s="16"/>
-      <c r="D44" s="16"/>
-      <c r="E44" s="16"/>
-      <c r="F44" s="16"/>
+      <c r="C44" s="13"/>
+      <c r="D44" s="13"/>
+      <c r="E44" s="13"/>
+      <c r="F44" s="13"/>
       <c r="G44" s="2">
         <v>10</v>
       </c>
@@ -1663,10 +1726,10 @@
       </c>
     </row>
     <row r="45" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C45" s="16"/>
-      <c r="D45" s="16"/>
-      <c r="E45" s="16"/>
-      <c r="F45" s="16"/>
+      <c r="C45" s="13"/>
+      <c r="D45" s="13"/>
+      <c r="E45" s="13"/>
+      <c r="F45" s="13"/>
       <c r="G45" s="2">
         <v>11</v>
       </c>
@@ -2100,13 +2163,13 @@
       </c>
     </row>
     <row r="74" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G74" s="17" t="s">
+      <c r="G74" s="15" t="s">
         <v>90</v>
       </c>
-      <c r="H74" s="18"/>
-      <c r="I74" s="18"/>
-      <c r="J74" s="18"/>
-      <c r="K74" s="19"/>
+      <c r="H74" s="16"/>
+      <c r="I74" s="16"/>
+      <c r="J74" s="16"/>
+      <c r="K74" s="17"/>
     </row>
     <row r="75" spans="7:11" x14ac:dyDescent="0.25">
       <c r="G75" s="4" t="s">
@@ -2311,13 +2374,13 @@
       </c>
     </row>
     <row r="88" spans="7:11" x14ac:dyDescent="0.25">
-      <c r="G88" s="17" t="s">
+      <c r="G88" s="15" t="s">
         <v>91</v>
       </c>
-      <c r="H88" s="18"/>
-      <c r="I88" s="18"/>
-      <c r="J88" s="18"/>
-      <c r="K88" s="19"/>
+      <c r="H88" s="16"/>
+      <c r="I88" s="16"/>
+      <c r="J88" s="16"/>
+      <c r="K88" s="17"/>
     </row>
     <row r="89" spans="7:11" x14ac:dyDescent="0.25">
       <c r="G89" s="4" t="s">
@@ -2346,7 +2409,7 @@
       <c r="I90" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="J90" s="12" t="s">
+      <c r="J90" s="18" t="s">
         <v>84</v>
       </c>
       <c r="K90" s="8" t="s">
@@ -2363,7 +2426,7 @@
       <c r="I91" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="J91" s="13"/>
+      <c r="J91" s="19"/>
       <c r="K91" s="8" t="s">
         <v>86</v>
       </c>
@@ -2419,19 +2482,199 @@
         <v>23</v>
       </c>
     </row>
+    <row r="96" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="G96" s="15" t="s">
+        <v>129</v>
+      </c>
+      <c r="H96" s="16"/>
+      <c r="I96" s="16"/>
+      <c r="J96" s="16"/>
+      <c r="K96" s="17"/>
+    </row>
+    <row r="97" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="G97" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H97" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I97" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="J97" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="K97" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="98" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="G98" s="20">
+        <v>1</v>
+      </c>
+      <c r="H98" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I98" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="J98" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="K98" s="20" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="99" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="G99" s="20">
+        <v>2</v>
+      </c>
+      <c r="H99" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="I99" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="J99" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="K99" s="20" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="100" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="G100" s="20">
+        <v>3</v>
+      </c>
+      <c r="H100" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="I100" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="J100" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="K100" s="10" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="101" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="G101" s="20">
+        <v>4</v>
+      </c>
+      <c r="H101" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="I101" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="J101" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="K101" s="10" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="102" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="G102" s="20">
+        <v>5</v>
+      </c>
+      <c r="H102" s="10" t="s">
+        <v>133</v>
+      </c>
+      <c r="I102" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="J102" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="K102" s="10" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="103" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="G103" s="20">
+        <v>6</v>
+      </c>
+      <c r="H103" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="I103" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="J103" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="K103" s="10" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="104" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="G104" s="20">
+        <v>7</v>
+      </c>
+      <c r="H104" s="10" t="s">
+        <v>135</v>
+      </c>
+      <c r="I104" s="10" t="s">
+        <v>139</v>
+      </c>
+      <c r="J104" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="K104" s="10" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="105" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="G105" s="20">
+        <v>8</v>
+      </c>
+      <c r="H105" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="I105" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="J105" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="K105" s="10" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="106" spans="7:11" x14ac:dyDescent="0.25">
+      <c r="G106" s="20">
+        <v>9</v>
+      </c>
+      <c r="H106" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="I106" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="J106" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="K106" s="10" t="s">
+        <v>148</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="11">
-    <mergeCell ref="C33:F45"/>
-    <mergeCell ref="G47:K47"/>
-    <mergeCell ref="G63:K63"/>
-    <mergeCell ref="G74:K74"/>
-    <mergeCell ref="G88:K88"/>
+  <mergeCells count="12">
+    <mergeCell ref="G96:K96"/>
     <mergeCell ref="J90:J91"/>
     <mergeCell ref="G33:K33"/>
     <mergeCell ref="G1:K1"/>
     <mergeCell ref="G7:K7"/>
     <mergeCell ref="G13:K13"/>
     <mergeCell ref="G19:K19"/>
+    <mergeCell ref="C33:F45"/>
+    <mergeCell ref="G47:K47"/>
+    <mergeCell ref="G63:K63"/>
+    <mergeCell ref="G74:K74"/>
+    <mergeCell ref="G88:K88"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>